<commit_message>
BC mass balance fix
</commit_message>
<xml_diff>
--- a/forecast/CVP-ops/MAR50_WY2018v.xlsx
+++ b/forecast/CVP-ops/MAR50_WY2018v.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\RMA_Project_Data\USBR-TempModeling\WTMP Git\UpperSac-ForecastingWorkshop\forecast\CVP-ops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\WTMP\WTMP_Studies\WTMP_SacramentoTrinity_Ben\forecast\CVP-ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EA2F50-8B03-4EBD-91C5-A3FC64C3F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518F8AAD-C865-4C83-8C67-EA9146CD676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A8BA9C2-AFB9-4A45-B4E0-ABDCB1C8E7FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A8BA9C2-AFB9-4A45-B4E0-ABDCB1C8E7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Mar50_WY2018" sheetId="1" r:id="rId1"/>
@@ -720,13 +720,13 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>203.7</c:v>
+                  <c:v>203.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>117.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111.3</c:v>
+                  <c:v>111.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>137.19999999999999</c:v>
@@ -735,16 +735,16 @@
                   <c:v>127.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.9</c:v>
+                  <c:v>48.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.2</c:v>
+                  <c:v>43.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.7</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>18.2</c:v>
@@ -7448,9 +7448,9 @@
   <dimension ref="A1:AA293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B26" sqref="B26"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7669,13 +7669,13 @@
         <v>72</v>
       </c>
       <c r="E7" s="6">
-        <v>203.7</v>
+        <v>203.6</v>
       </c>
       <c r="F7" s="6">
         <v>117.6</v>
       </c>
       <c r="G7" s="6">
-        <v>111.3</v>
+        <v>111.4</v>
       </c>
       <c r="H7" s="6">
         <v>137.19999999999999</v>
@@ -7684,16 +7684,16 @@
         <v>127.7</v>
       </c>
       <c r="J7" s="6">
-        <v>48.9</v>
+        <v>48.8</v>
       </c>
       <c r="K7" s="6">
-        <v>43.2</v>
+        <v>43.1</v>
       </c>
       <c r="L7" s="6">
         <v>27</v>
       </c>
       <c r="M7" s="6">
-        <v>18.7</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="N7" s="6">
         <v>18.2</v>

</xml_diff>